<commit_message>
Don't make result calculations mandatory
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-calculation-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-calculation-validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2C2DE0-36CC-5742-B1F8-651958F4C426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2078805F-AE7B-D04A-9567-884BFE1833A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>